<commit_message>
Ajout du TI du jour
</commit_message>
<xml_diff>
--- a/Excel/TI/Mon_TI_2024_03_06.xlsx
+++ b/Excel/TI/Mon_TI_2024_03_06.xlsx
@@ -648,13 +648,13 @@
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="n">
-        <v>48.2</v>
+        <v>45.4</v>
       </c>
       <c r="G2" t="n">
-        <v>44.3</v>
+        <v>44.1</v>
       </c>
       <c r="H2" t="n">
-        <v>41.3</v>
+        <v>41.2</v>
       </c>
       <c r="I2" t="n">
         <v>9</v>
@@ -672,19 +672,19 @@
         <v>7</v>
       </c>
       <c r="N2" t="n">
+        <v>38</v>
+      </c>
+      <c r="O2" t="n">
         <v>40</v>
       </c>
-      <c r="O2" t="n">
+      <c r="P2" t="n">
         <v>44</v>
       </c>
-      <c r="P2" t="n">
+      <c r="Q2" t="n">
         <v>55</v>
       </c>
-      <c r="Q2" t="n">
+      <c r="R2" t="n">
         <v>50</v>
-      </c>
-      <c r="R2" t="n">
-        <v>52</v>
       </c>
       <c r="S2" t="inlineStr">
         <is>
@@ -768,7 +768,7 @@
         </is>
       </c>
       <c r="AJ2" t="n">
-        <v>-1.9</v>
+        <v>-1.8</v>
       </c>
       <c r="AK2" t="inlineStr"/>
       <c r="AL2" t="inlineStr"/>
@@ -781,17 +781,13 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Donovan Mitchell</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Day-To-Day</t>
-        </is>
-      </c>
+          <t>Jarrett Allen</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
-          <t>G</t>
+          <t>C</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -800,82 +796,78 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>38.4</v>
+        <v>32</v>
       </c>
       <c r="G3" t="n">
-        <v>41.1</v>
+        <v>34.7</v>
       </c>
       <c r="H3" t="n">
-        <v>39.9</v>
+        <v>33.8</v>
       </c>
       <c r="I3" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="J3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L3" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="M3" t="n">
-        <v>6</v>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>2</v>
+      </c>
+      <c r="N3" t="n">
+        <v>41</v>
+      </c>
+      <c r="O3" t="n">
+        <v>35</v>
       </c>
       <c r="P3" t="n">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="Q3" t="n">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="R3" t="n">
+        <v>37</v>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>ATL</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="V3" t="n">
+        <v>35</v>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="X3" t="n">
+        <v>50</v>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="Z3" t="n">
         <v>26</v>
       </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>ATL</t>
-        </is>
-      </c>
-      <c r="U3" t="inlineStr">
-        <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="V3" t="n">
-        <v>27</v>
-      </c>
-      <c r="W3" t="inlineStr">
-        <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="X3" t="n">
-        <v>37</v>
-      </c>
-      <c r="Y3" t="inlineStr">
-        <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="Z3" t="n">
-        <v>61</v>
-      </c>
       <c r="AA3" t="inlineStr">
         <is>
           <t>vs</t>
@@ -922,13 +914,13 @@
         </is>
       </c>
       <c r="AJ3" t="n">
-        <v>-3.8</v>
+        <v>-1.7</v>
       </c>
       <c r="AK3" t="n">
-        <v>-13.3</v>
+        <v>-7.9</v>
       </c>
       <c r="AL3" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4">
@@ -942,11 +934,7 @@
           <t>De'Aaron Fox</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Questionable</t>
-        </is>
-      </c>
+      <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
           <t>G</t>
@@ -954,22 +942,22 @@
       </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="n">
-        <v>46</v>
+        <v>40.8</v>
       </c>
       <c r="G4" t="n">
-        <v>35</v>
+        <v>33.7</v>
       </c>
       <c r="H4" t="n">
-        <v>35.9</v>
+        <v>35.7</v>
       </c>
       <c r="I4" t="n">
         <v>9</v>
       </c>
       <c r="J4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L4" t="n">
         <v>1</v>
@@ -977,24 +965,24 @@
       <c r="M4" t="n">
         <v>4</v>
       </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="N4" t="n">
+        <v>25</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="P4" t="n">
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Q4" t="n">
         <v>37</v>
       </c>
-      <c r="Q4" t="n">
+      <c r="R4" t="n">
         <v>52</v>
-      </c>
-      <c r="R4" t="n">
-        <v>46</v>
       </c>
       <c r="S4" t="inlineStr">
         <is>
@@ -1078,7 +1066,7 @@
         </is>
       </c>
       <c r="AJ4" t="n">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="AK4" t="inlineStr"/>
       <c r="AL4" t="inlineStr"/>
@@ -1086,12 +1074,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>PHI</t>
+          <t>LAC</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Tyrese Maxey</t>
+          <t>James Harden</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
@@ -1100,19 +1088,15 @@
           <t>G</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>O</t>
-        </is>
-      </c>
+      <c r="E5" t="inlineStr"/>
       <c r="F5" t="n">
-        <v>37.8</v>
+        <v>33</v>
       </c>
       <c r="G5" t="n">
-        <v>34.7</v>
+        <v>33.1</v>
       </c>
       <c r="H5" t="n">
-        <v>35.9</v>
+        <v>31.8</v>
       </c>
       <c r="I5" t="n">
         <v>11</v>
@@ -1121,48 +1105,46 @@
         <v>2</v>
       </c>
       <c r="K5" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L5" t="n">
+        <v>2</v>
+      </c>
+      <c r="M5" t="n">
         <v>3</v>
       </c>
-      <c r="M5" t="n">
-        <v>5</v>
-      </c>
       <c r="N5" t="n">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="O5" t="n">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="P5" t="n">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="Q5" t="n">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="R5" t="n">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="V5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="V5" t="n">
+        <v>48</v>
       </c>
       <c r="W5" t="inlineStr">
         <is>
@@ -1191,27 +1173,27 @@
       </c>
       <c r="AB5" t="inlineStr">
         <is>
-          <t>NOP</t>
+          <t>CHI</t>
         </is>
       </c>
       <c r="AC5" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AD5" t="inlineStr">
         <is>
-          <t>NYK</t>
+          <t>MIL</t>
         </is>
       </c>
       <c r="AE5" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AF5" t="inlineStr">
         <is>
-          <t>NYK</t>
+          <t>MIN</t>
         </is>
       </c>
       <c r="AG5" t="inlineStr">
@@ -1221,23 +1203,19 @@
       </c>
       <c r="AH5" t="inlineStr">
         <is>
-          <t>MIL</t>
+          <t>CHI</t>
         </is>
       </c>
       <c r="AI5" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AJ5" t="n">
-        <v>-0.2</v>
-      </c>
-      <c r="AK5" t="n">
-        <v>-8.800000000000001</v>
-      </c>
-      <c r="AL5" t="n">
-        <v>9</v>
-      </c>
+        <v>-0.7</v>
+      </c>
+      <c r="AK5" t="inlineStr"/>
+      <c r="AL5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1262,13 +1240,13 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>36.4</v>
+        <v>34.6</v>
       </c>
       <c r="G6" t="n">
-        <v>33.9</v>
+        <v>32.5</v>
       </c>
       <c r="H6" t="n">
-        <v>30.9</v>
+        <v>31</v>
       </c>
       <c r="I6" t="n">
         <v>9</v>
@@ -1277,28 +1255,28 @@
         <v>1</v>
       </c>
       <c r="K6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M6" t="n">
         <v>4</v>
       </c>
       <c r="N6" t="n">
+        <v>34</v>
+      </c>
+      <c r="O6" t="n">
         <v>31</v>
       </c>
-      <c r="O6" t="n">
+      <c r="P6" t="n">
         <v>40</v>
       </c>
-      <c r="P6" t="n">
+      <c r="Q6" t="n">
         <v>23</v>
       </c>
-      <c r="Q6" t="n">
+      <c r="R6" t="n">
         <v>45</v>
-      </c>
-      <c r="R6" t="n">
-        <v>43</v>
       </c>
       <c r="S6" t="inlineStr">
         <is>
@@ -1380,7 +1358,7 @@
         </is>
       </c>
       <c r="AJ6" t="n">
-        <v>1.2</v>
+        <v>1.1</v>
       </c>
       <c r="AK6" t="n">
         <v>-4.2</v>
@@ -1392,63 +1370,59 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>CLE</t>
+          <t>MIL</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Evan Mobley</t>
+          <t>Damian Lillard</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr">
         <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>O</t>
-        </is>
-      </c>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
       <c r="F7" t="n">
-        <v>38.6</v>
+        <v>36</v>
       </c>
       <c r="G7" t="n">
-        <v>33.8</v>
+        <v>32.1</v>
       </c>
       <c r="H7" t="n">
-        <v>32.8</v>
+        <v>35.2</v>
       </c>
       <c r="I7" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="J7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K7" t="n">
         <v>3</v>
       </c>
       <c r="L7" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M7" t="n">
         <v>4</v>
       </c>
       <c r="N7" t="n">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="O7" t="n">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="P7" t="n">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="Q7" t="n">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="R7" t="n">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="S7" t="inlineStr">
         <is>
@@ -1457,7 +1431,7 @@
       </c>
       <c r="T7" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>GSW</t>
         </is>
       </c>
       <c r="U7" t="inlineStr">
@@ -1466,7 +1440,7 @@
         </is>
       </c>
       <c r="V7" t="n">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="W7" t="inlineStr">
         <is>
@@ -1490,42 +1464,42 @@
       </c>
       <c r="AA7" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AB7" t="inlineStr">
         <is>
-          <t>MIN</t>
+          <t>LAL</t>
         </is>
       </c>
       <c r="AC7" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AD7" t="inlineStr">
         <is>
-          <t>BKN</t>
+          <t>LAC</t>
         </is>
       </c>
       <c r="AE7" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AF7" t="inlineStr">
         <is>
-          <t>PHX</t>
+          <t>SAC</t>
         </is>
       </c>
       <c r="AG7" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AH7" t="inlineStr">
         <is>
-          <t>NOP</t>
+          <t>PHI</t>
         </is>
       </c>
       <c r="AI7" t="inlineStr">
@@ -1534,109 +1508,107 @@
         </is>
       </c>
       <c r="AJ7" t="n">
-        <v>1.6</v>
-      </c>
-      <c r="AK7" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="AL7" t="n">
-        <v>7</v>
-      </c>
+        <v>-2.1</v>
+      </c>
+      <c r="AK7" t="inlineStr"/>
+      <c r="AL7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>CLE</t>
+          <t>GSW</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Jarrett Allen</t>
+          <t>Stephen Curry</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
         <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>O</t>
-        </is>
-      </c>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr"/>
       <c r="F8" t="n">
-        <v>32</v>
+        <v>15.6</v>
       </c>
       <c r="G8" t="n">
-        <v>33.6</v>
+        <v>30.7</v>
       </c>
       <c r="H8" t="n">
-        <v>33.6</v>
+        <v>34.4</v>
       </c>
       <c r="I8" t="n">
         <v>13</v>
       </c>
       <c r="J8" t="n">
+        <v>6</v>
+      </c>
+      <c r="K8" t="n">
         <v>1</v>
       </c>
-      <c r="K8" t="n">
-        <v>2</v>
-      </c>
       <c r="L8" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="M8" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="N8" t="n">
-        <v>35</v>
+        <v>-12</v>
       </c>
       <c r="O8" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P8" t="n">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="Q8" t="n">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="R8" t="n">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="S8" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="T8" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>MIL</t>
         </is>
       </c>
       <c r="U8" t="inlineStr">
         <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="V8" t="n">
-        <v>35</v>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="V8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="W8" t="inlineStr">
         <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="X8" t="n">
-        <v>50</v>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="X8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="Y8" t="inlineStr">
         <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="Z8" t="n">
-        <v>26</v>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Z8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="AA8" t="inlineStr">
         <is>
@@ -1645,7 +1617,7 @@
       </c>
       <c r="AB8" t="inlineStr">
         <is>
-          <t>MIN</t>
+          <t>CHI</t>
         </is>
       </c>
       <c r="AC8" t="inlineStr">
@@ -1655,17 +1627,17 @@
       </c>
       <c r="AD8" t="inlineStr">
         <is>
-          <t>BKN</t>
+          <t>SAS</t>
         </is>
       </c>
       <c r="AE8" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AF8" t="inlineStr">
         <is>
-          <t>PHX</t>
+          <t>SAS</t>
         </is>
       </c>
       <c r="AG8" t="inlineStr">
@@ -1675,88 +1647,76 @@
       </c>
       <c r="AH8" t="inlineStr">
         <is>
-          <t>NOP</t>
+          <t>DAL</t>
         </is>
       </c>
       <c r="AI8" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AJ8" t="n">
-        <v>-1.5</v>
-      </c>
-      <c r="AK8" t="n">
-        <v>-7.7</v>
-      </c>
-      <c r="AL8" t="n">
-        <v>8</v>
-      </c>
+        <v>1.7</v>
+      </c>
+      <c r="AK8" t="inlineStr"/>
+      <c r="AL8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>POR</t>
+          <t>LAL</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Deandre Ayton</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Questionable</t>
-        </is>
-      </c>
+          <t>Austin Reaves</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>G</t>
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="n">
-        <v>36.4</v>
+        <v>26.8</v>
       </c>
       <c r="G9" t="n">
-        <v>33.2</v>
+        <v>29.9</v>
       </c>
       <c r="H9" t="n">
-        <v>29.2</v>
+        <v>25.3</v>
       </c>
       <c r="I9" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="J9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K9" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L9" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M9" t="n">
-        <v>4</v>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>2</v>
+      </c>
+      <c r="N9" t="n">
+        <v>32</v>
+      </c>
+      <c r="O9" t="n">
+        <v>37</v>
       </c>
       <c r="P9" t="n">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="Q9" t="n">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="R9" t="n">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="S9" t="inlineStr">
         <is>
@@ -1765,24 +1725,24 @@
       </c>
       <c r="T9" t="inlineStr">
         <is>
-          <t>OKC</t>
+          <t>SAC</t>
         </is>
       </c>
       <c r="U9" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="V9" t="n">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="W9" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="X9" t="n">
-        <v>21</v>
+        <v>-7</v>
       </c>
       <c r="Y9" t="inlineStr">
         <is>
@@ -1801,7 +1761,7 @@
       </c>
       <c r="AB9" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>MIL</t>
         </is>
       </c>
       <c r="AC9" t="inlineStr">
@@ -1811,17 +1771,17 @@
       </c>
       <c r="AD9" t="inlineStr">
         <is>
-          <t>TOR</t>
+          <t>MIN</t>
         </is>
       </c>
       <c r="AE9" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AF9" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>SAC</t>
         </is>
       </c>
       <c r="AG9" t="inlineStr">
@@ -1831,7 +1791,7 @@
       </c>
       <c r="AH9" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>GSW</t>
         </is>
       </c>
       <c r="AI9" t="inlineStr">
@@ -1840,7 +1800,7 @@
         </is>
       </c>
       <c r="AJ9" t="n">
-        <v>0.5</v>
+        <v>1.3</v>
       </c>
       <c r="AK9" t="inlineStr"/>
       <c r="AL9" t="inlineStr"/>
@@ -1848,145 +1808,145 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>LAC</t>
+          <t>WAS</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>James Harden</t>
+          <t>Deni Avdija</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr">
         <is>
-          <t>G</t>
+          <t>F</t>
         </is>
       </c>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="n">
-        <v>28</v>
+        <v>29.8</v>
       </c>
       <c r="G10" t="n">
-        <v>31.9</v>
+        <v>28.7</v>
       </c>
       <c r="H10" t="n">
-        <v>31.6</v>
+        <v>24.4</v>
       </c>
       <c r="I10" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="J10" t="n">
+        <v>3</v>
+      </c>
+      <c r="K10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L10" t="n">
+        <v>3</v>
+      </c>
+      <c r="M10" t="n">
         <v>2</v>
       </c>
-      <c r="K10" t="n">
-        <v>4</v>
-      </c>
-      <c r="L10" t="n">
-        <v>2</v>
-      </c>
-      <c r="M10" t="n">
-        <v>4</v>
-      </c>
       <c r="N10" t="n">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="O10" t="n">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="P10" t="n">
-        <v>31</v>
-      </c>
-      <c r="Q10" t="n">
-        <v>29</v>
-      </c>
-      <c r="R10" t="n">
-        <v>19</v>
+        <v>37</v>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="S10" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="T10" t="inlineStr">
         <is>
+          <t>ORL</t>
+        </is>
+      </c>
+      <c r="U10" t="inlineStr">
+        <is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="V10" t="n">
+        <v>3</v>
+      </c>
+      <c r="W10" t="inlineStr">
+        <is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="X10" t="n">
+        <v>11</v>
+      </c>
+      <c r="Y10" t="inlineStr">
+        <is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="Z10" t="n">
+        <v>41</v>
+      </c>
+      <c r="AA10" t="inlineStr">
+        <is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="AB10" t="inlineStr">
+        <is>
+          <t>CHA</t>
+        </is>
+      </c>
+      <c r="AC10" t="inlineStr">
+        <is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="AD10" t="inlineStr">
+        <is>
+          <t>MIA</t>
+        </is>
+      </c>
+      <c r="AE10" t="inlineStr">
+        <is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="AF10" t="inlineStr">
+        <is>
+          <t>MEM</t>
+        </is>
+      </c>
+      <c r="AG10" t="inlineStr">
+        <is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="AH10" t="inlineStr">
+        <is>
           <t>HOU</t>
         </is>
       </c>
-      <c r="U10" t="inlineStr">
-        <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="V10" t="n">
-        <v>48</v>
-      </c>
-      <c r="W10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="X10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="Y10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="Z10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AA10" t="inlineStr">
-        <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="AB10" t="inlineStr">
-        <is>
-          <t>CHI</t>
-        </is>
-      </c>
-      <c r="AC10" t="inlineStr">
-        <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="AD10" t="inlineStr">
-        <is>
-          <t>MIL</t>
-        </is>
-      </c>
-      <c r="AE10" t="inlineStr">
-        <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="AF10" t="inlineStr">
-        <is>
-          <t>MIN</t>
-        </is>
-      </c>
-      <c r="AG10" t="inlineStr">
-        <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="AH10" t="inlineStr">
-        <is>
-          <t>CHI</t>
-        </is>
-      </c>
       <c r="AI10" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AJ10" t="n">
-        <v>-1</v>
+        <v>-0.3</v>
       </c>
       <c r="AK10" t="inlineStr"/>
       <c r="AL10" t="inlineStr"/>
@@ -2014,19 +1974,19 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>24.6</v>
+        <v>21.8</v>
       </c>
       <c r="G11" t="n">
-        <v>30.9</v>
+        <v>28.7</v>
       </c>
       <c r="H11" t="n">
-        <v>30.1</v>
+        <v>29.5</v>
       </c>
       <c r="I11" t="n">
         <v>12</v>
       </c>
       <c r="J11" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K11" t="n">
         <v>4</v>
@@ -2035,22 +1995,22 @@
         <v>2</v>
       </c>
       <c r="M11" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N11" t="n">
+        <v>1</v>
+      </c>
+      <c r="O11" t="n">
         <v>21</v>
       </c>
-      <c r="O11" t="n">
+      <c r="P11" t="n">
         <v>22</v>
       </c>
-      <c r="P11" t="n">
+      <c r="Q11" t="n">
         <v>37</v>
       </c>
-      <c r="Q11" t="n">
+      <c r="R11" t="n">
         <v>28</v>
-      </c>
-      <c r="R11" t="n">
-        <v>15</v>
       </c>
       <c r="S11" t="inlineStr">
         <is>
@@ -2132,10 +2092,10 @@
         </is>
       </c>
       <c r="AJ11" t="n">
-        <v>-2.8</v>
+        <v>-3.2</v>
       </c>
       <c r="AK11" t="n">
-        <v>-2.4</v>
+        <v>-1.7</v>
       </c>
       <c r="AL11" t="n">
         <v>11</v>
@@ -2144,59 +2104,65 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>GSW</t>
+          <t>POR</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Stephen Curry</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr"/>
+          <t>Jerami Grant</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Questionable</t>
+        </is>
+      </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>G</t>
+          <t>F</t>
         </is>
       </c>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="n">
-        <v>15.6</v>
+        <v>19.8</v>
       </c>
       <c r="G12" t="n">
-        <v>30.7</v>
+        <v>27.9</v>
       </c>
       <c r="H12" t="n">
-        <v>34.4</v>
+        <v>27.9</v>
       </c>
       <c r="I12" t="n">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="J12" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="K12" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L12" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" t="n">
         <v>2</v>
       </c>
-      <c r="M12" t="n">
-        <v>5</v>
-      </c>
-      <c r="N12" t="n">
-        <v>-12</v>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="O12" t="n">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="P12" t="n">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="Q12" t="n">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="R12" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="S12" t="inlineStr">
         <is>
@@ -2205,38 +2171,32 @@
       </c>
       <c r="T12" t="inlineStr">
         <is>
-          <t>MIL</t>
+          <t>OKC</t>
         </is>
       </c>
       <c r="U12" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="V12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="V12" t="n">
+        <v>30</v>
       </c>
       <c r="W12" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="X12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="X12" t="n">
+        <v>12</v>
       </c>
       <c r="Y12" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="Z12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="Z12" t="n">
+        <v>11</v>
       </c>
       <c r="AA12" t="inlineStr">
         <is>
@@ -2245,7 +2205,7 @@
       </c>
       <c r="AB12" t="inlineStr">
         <is>
-          <t>CHI</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="AC12" t="inlineStr">
@@ -2255,27 +2215,27 @@
       </c>
       <c r="AD12" t="inlineStr">
         <is>
-          <t>SAS</t>
+          <t>TOR</t>
         </is>
       </c>
       <c r="AE12" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AF12" t="inlineStr">
         <is>
-          <t>SAS</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="AG12" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AH12" t="inlineStr">
         <is>
-          <t>DAL</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="AI12" t="inlineStr">
@@ -2284,7 +2244,7 @@
         </is>
       </c>
       <c r="AJ12" t="n">
-        <v>1.7</v>
+        <v>4.3</v>
       </c>
       <c r="AK12" t="inlineStr"/>
       <c r="AL12" t="inlineStr"/>
@@ -2292,97 +2252,85 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>LAL</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Jaren Jackson Jr.</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Doubtful</t>
-        </is>
-      </c>
+          <t>D'Angelo Russell</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>G</t>
         </is>
       </c>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="n">
-        <v>30.4</v>
+        <v>28.8</v>
       </c>
       <c r="G13" t="n">
-        <v>30.5</v>
+        <v>27.8</v>
       </c>
       <c r="H13" t="n">
-        <v>30.5</v>
+        <v>25.9</v>
       </c>
       <c r="I13" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="J13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K13" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L13" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M13" t="n">
         <v>1</v>
       </c>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="O13" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="N13" t="n">
+        <v>38</v>
+      </c>
+      <c r="O13" t="n">
+        <v>22</v>
       </c>
       <c r="P13" t="n">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="Q13" t="n">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="R13" t="n">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="S13" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="T13" t="inlineStr">
         <is>
-          <t>PHI</t>
+          <t>SAC</t>
         </is>
       </c>
       <c r="U13" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="V13" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="V13" t="n">
+        <v>43</v>
       </c>
       <c r="W13" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="X13" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="X13" t="n">
+        <v>28</v>
       </c>
       <c r="Y13" t="inlineStr">
         <is>
@@ -2401,27 +2349,27 @@
       </c>
       <c r="AB13" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>MIL</t>
         </is>
       </c>
       <c r="AC13" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AD13" t="inlineStr">
         <is>
-          <t>OKC</t>
+          <t>MIN</t>
         </is>
       </c>
       <c r="AE13" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AF13" t="inlineStr">
         <is>
-          <t>WAS</t>
+          <t>SAC</t>
         </is>
       </c>
       <c r="AG13" t="inlineStr">
@@ -2431,16 +2379,16 @@
       </c>
       <c r="AH13" t="inlineStr">
         <is>
-          <t>CHA</t>
+          <t>GSW</t>
         </is>
       </c>
       <c r="AI13" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AJ13" t="n">
-        <v>2.4</v>
+        <v>0.9</v>
       </c>
       <c r="AK13" t="inlineStr"/>
       <c r="AL13" t="inlineStr"/>
@@ -2448,12 +2396,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>WAS</t>
+          <t>PHI</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Deni Avdija</t>
+          <t>Tobias Harris</t>
         </is>
       </c>
       <c r="C14" t="inlineStr"/>
@@ -2462,51 +2410,49 @@
           <t>F</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr"/>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
       <c r="F14" t="n">
-        <v>32.6</v>
+        <v>28.6</v>
       </c>
       <c r="G14" t="n">
-        <v>30.4</v>
+        <v>27.4</v>
       </c>
       <c r="H14" t="n">
-        <v>24.5</v>
+        <v>28.7</v>
       </c>
       <c r="I14" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J14" t="n">
+        <v>4</v>
+      </c>
+      <c r="K14" t="n">
+        <v>3</v>
+      </c>
+      <c r="L14" t="n">
         <v>2</v>
       </c>
-      <c r="K14" t="n">
+      <c r="M14" t="n">
         <v>1</v>
       </c>
-      <c r="L14" t="n">
-        <v>4</v>
-      </c>
-      <c r="M14" t="n">
-        <v>2</v>
-      </c>
       <c r="N14" t="n">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="O14" t="n">
-        <v>37</v>
-      </c>
-      <c r="P14" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="Q14" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="R14" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>39</v>
+      </c>
+      <c r="P14" t="n">
+        <v>59</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>3</v>
+      </c>
+      <c r="R14" t="n">
+        <v>14</v>
       </c>
       <c r="S14" t="inlineStr">
         <is>
@@ -2515,32 +2461,38 @@
       </c>
       <c r="T14" t="inlineStr">
         <is>
-          <t>ORL</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="U14" t="inlineStr">
         <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="V14" t="n">
-        <v>3</v>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="V14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="W14" t="inlineStr">
         <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="X14" t="n">
-        <v>11</v>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="X14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="Y14" t="inlineStr">
         <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="Z14" t="n">
-        <v>41</v>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Z14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="AA14" t="inlineStr">
         <is>
@@ -2549,7 +2501,7 @@
       </c>
       <c r="AB14" t="inlineStr">
         <is>
-          <t>CHA</t>
+          <t>NOP</t>
         </is>
       </c>
       <c r="AC14" t="inlineStr">
@@ -2559,7 +2511,7 @@
       </c>
       <c r="AD14" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>NYK</t>
         </is>
       </c>
       <c r="AE14" t="inlineStr">
@@ -2569,7 +2521,7 @@
       </c>
       <c r="AF14" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>NYK</t>
         </is>
       </c>
       <c r="AG14" t="inlineStr">
@@ -2579,7 +2531,7 @@
       </c>
       <c r="AH14" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>MIL</t>
         </is>
       </c>
       <c r="AI14" t="inlineStr">
@@ -2588,85 +2540,97 @@
         </is>
       </c>
       <c r="AJ14" t="n">
-        <v>-0.4</v>
-      </c>
-      <c r="AK14" t="inlineStr"/>
-      <c r="AL14" t="inlineStr"/>
+        <v>0.4</v>
+      </c>
+      <c r="AK14" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="AL14" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>MIL</t>
+          <t>GSW</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Damian Lillard</t>
+          <t>Andrew Wiggins</t>
         </is>
       </c>
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr">
         <is>
-          <t>G</t>
+          <t>F</t>
         </is>
       </c>
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="n">
-        <v>30.2</v>
+        <v>25.4</v>
       </c>
       <c r="G15" t="n">
-        <v>29.2</v>
+        <v>25.1</v>
       </c>
       <c r="H15" t="n">
-        <v>34.8</v>
+        <v>17.8</v>
       </c>
       <c r="I15" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J15" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K15" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L15" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M15" t="n">
-        <v>3</v>
-      </c>
-      <c r="N15" t="n">
-        <v>14</v>
-      </c>
-      <c r="O15" t="n">
-        <v>24</v>
-      </c>
-      <c r="P15" t="n">
-        <v>40</v>
-      </c>
-      <c r="Q15" t="n">
-        <v>42</v>
+        <v>0</v>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="R15" t="n">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="S15" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="T15" t="inlineStr">
         <is>
-          <t>GSW</t>
+          <t>MIL</t>
         </is>
       </c>
       <c r="U15" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="V15" t="n">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="W15" t="inlineStr">
         <is>
@@ -2690,22 +2654,22 @@
       </c>
       <c r="AA15" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AB15" t="inlineStr">
         <is>
-          <t>LAL</t>
+          <t>CHI</t>
         </is>
       </c>
       <c r="AC15" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AD15" t="inlineStr">
         <is>
-          <t>LAC</t>
+          <t>SAS</t>
         </is>
       </c>
       <c r="AE15" t="inlineStr">
@@ -2715,26 +2679,26 @@
       </c>
       <c r="AF15" t="inlineStr">
         <is>
-          <t>SAC</t>
+          <t>SAS</t>
         </is>
       </c>
       <c r="AG15" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AH15" t="inlineStr">
         <is>
-          <t>PHI</t>
+          <t>DAL</t>
         </is>
       </c>
       <c r="AI15" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AJ15" t="n">
-        <v>-1.7</v>
+        <v>-0.5</v>
       </c>
       <c r="AK15" t="inlineStr"/>
       <c r="AL15" t="inlineStr"/>
@@ -2742,68 +2706,72 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>LAL</t>
+          <t>LAC</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Austin Reaves</t>
+          <t>Paul George</t>
         </is>
       </c>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr">
         <is>
-          <t>G</t>
+          <t>F</t>
         </is>
       </c>
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="n">
-        <v>23.6</v>
+        <v>23.4</v>
       </c>
       <c r="G16" t="n">
-        <v>28.5</v>
+        <v>24.3</v>
       </c>
       <c r="H16" t="n">
-        <v>25.2</v>
+        <v>30.6</v>
       </c>
       <c r="I16" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="J16" t="n">
         <v>3</v>
       </c>
       <c r="K16" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L16" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N16" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="O16" t="n">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="P16" t="n">
-        <v>25</v>
-      </c>
-      <c r="Q16" t="n">
-        <v>18</v>
-      </c>
-      <c r="R16" t="n">
-        <v>16</v>
+        <v>33</v>
+      </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="S16" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="T16" t="inlineStr">
         <is>
-          <t>SAC</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="U16" t="inlineStr">
@@ -2812,15 +2780,17 @@
         </is>
       </c>
       <c r="V16" t="n">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="W16" t="inlineStr">
         <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="X16" t="n">
-        <v>-7</v>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="X16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="Y16" t="inlineStr">
         <is>
@@ -2839,46 +2809,46 @@
       </c>
       <c r="AB16" t="inlineStr">
         <is>
+          <t>CHI</t>
+        </is>
+      </c>
+      <c r="AC16" t="inlineStr">
+        <is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="AD16" t="inlineStr">
+        <is>
           <t>MIL</t>
         </is>
       </c>
-      <c r="AC16" t="inlineStr">
-        <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="AD16" t="inlineStr">
+      <c r="AE16" t="inlineStr">
+        <is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="AF16" t="inlineStr">
         <is>
           <t>MIN</t>
         </is>
       </c>
-      <c r="AE16" t="inlineStr">
-        <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="AF16" t="inlineStr">
-        <is>
-          <t>SAC</t>
-        </is>
-      </c>
       <c r="AG16" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AH16" t="inlineStr">
         <is>
-          <t>GSW</t>
+          <t>CHI</t>
         </is>
       </c>
       <c r="AI16" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AJ16" t="n">
-        <v>1.3</v>
+        <v>-0.5</v>
       </c>
       <c r="AK16" t="inlineStr"/>
       <c r="AL16" t="inlineStr"/>
@@ -2886,12 +2856,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>LAL</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>D'Angelo Russell</t>
+          <t>Fred VanVleet</t>
         </is>
       </c>
       <c r="C17" t="inlineStr"/>
@@ -2900,45 +2870,49 @@
           <t>G</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr"/>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
       <c r="F17" t="n">
-        <v>27.4</v>
+        <v>26.2</v>
       </c>
       <c r="G17" t="n">
-        <v>28</v>
+        <v>22.7</v>
       </c>
       <c r="H17" t="n">
-        <v>25.7</v>
+        <v>26.4</v>
       </c>
       <c r="I17" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="J17" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K17" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L17" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M17" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N17" t="n">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="O17" t="n">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="P17" t="n">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="Q17" t="n">
-        <v>31</v>
+        <v>-2</v>
       </c>
       <c r="R17" t="n">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="S17" t="inlineStr">
         <is>
@@ -2947,55 +2921,57 @@
       </c>
       <c r="T17" t="inlineStr">
         <is>
+          <t>LAC</t>
+        </is>
+      </c>
+      <c r="U17" t="inlineStr">
+        <is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="V17" t="n">
+        <v>38</v>
+      </c>
+      <c r="W17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="X17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Y17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Z17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AA17" t="inlineStr">
+        <is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="AB17" t="inlineStr">
+        <is>
+          <t>POR</t>
+        </is>
+      </c>
+      <c r="AC17" t="inlineStr">
+        <is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="AD17" t="inlineStr">
+        <is>
           <t>SAC</t>
         </is>
       </c>
-      <c r="U17" t="inlineStr">
-        <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="V17" t="n">
-        <v>43</v>
-      </c>
-      <c r="W17" t="inlineStr">
-        <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="X17" t="n">
-        <v>28</v>
-      </c>
-      <c r="Y17" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="Z17" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AA17" t="inlineStr">
-        <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="AB17" t="inlineStr">
-        <is>
-          <t>MIL</t>
-        </is>
-      </c>
-      <c r="AC17" t="inlineStr">
-        <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="AD17" t="inlineStr">
-        <is>
-          <t>MIN</t>
-        </is>
-      </c>
       <c r="AE17" t="inlineStr">
         <is>
           <t>@</t>
@@ -3003,7 +2979,7 @@
       </c>
       <c r="AF17" t="inlineStr">
         <is>
-          <t>SAC</t>
+          <t>SAS</t>
         </is>
       </c>
       <c r="AG17" t="inlineStr">
@@ -3013,7 +2989,7 @@
       </c>
       <c r="AH17" t="inlineStr">
         <is>
-          <t>GSW</t>
+          <t>WAS</t>
         </is>
       </c>
       <c r="AI17" t="inlineStr">
@@ -3022,27 +2998,27 @@
         </is>
       </c>
       <c r="AJ17" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="AK17" t="inlineStr"/>
-      <c r="AL17" t="inlineStr"/>
+        <v>-0.4</v>
+      </c>
+      <c r="AK17" t="n">
+        <v>-6.2</v>
+      </c>
+      <c r="AL17" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>POR</t>
+          <t>OKC</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Jerami Grant</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Doubtful</t>
-        </is>
-      </c>
+          <t>Gordon Hayward</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr">
         <is>
           <t>F</t>
@@ -3050,77 +3026,83 @@
       </c>
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="n">
-        <v>19.8</v>
+        <v>3.2</v>
       </c>
       <c r="G18" t="n">
-        <v>27.9</v>
+        <v>16</v>
       </c>
       <c r="H18" t="n">
-        <v>27.9</v>
+        <v>19.5</v>
       </c>
       <c r="I18" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="J18" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="K18" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L18" t="n">
         <v>0</v>
       </c>
       <c r="M18" t="n">
+        <v>0</v>
+      </c>
+      <c r="N18" t="n">
+        <v>1</v>
+      </c>
+      <c r="O18" t="n">
+        <v>5</v>
+      </c>
+      <c r="P18" t="n">
+        <v>-1</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>9</v>
+      </c>
+      <c r="R18" t="n">
         <v>2</v>
       </c>
-      <c r="N18" t="n">
-        <v>3</v>
-      </c>
-      <c r="O18" t="n">
-        <v>13</v>
-      </c>
-      <c r="P18" t="n">
-        <v>43</v>
-      </c>
-      <c r="Q18" t="n">
-        <v>11</v>
-      </c>
-      <c r="R18" t="n">
-        <v>29</v>
-      </c>
       <c r="S18" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="T18" t="inlineStr">
         <is>
-          <t>OKC</t>
+          <t>POR</t>
         </is>
       </c>
       <c r="U18" t="inlineStr">
         <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="V18" t="n">
-        <v>30</v>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="V18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="W18" t="inlineStr">
         <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="X18" t="n">
-        <v>12</v>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="X18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="Y18" t="inlineStr">
         <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="Z18" t="n">
-        <v>11</v>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Z18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="AA18" t="inlineStr">
         <is>
@@ -3129,7 +3111,7 @@
       </c>
       <c r="AB18" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="AC18" t="inlineStr">
@@ -3139,7 +3121,7 @@
       </c>
       <c r="AD18" t="inlineStr">
         <is>
-          <t>TOR</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="AE18" t="inlineStr">
@@ -3149,7 +3131,7 @@
       </c>
       <c r="AF18" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="AG18" t="inlineStr">
@@ -3159,16 +3141,16 @@
       </c>
       <c r="AH18" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>DAL</t>
         </is>
       </c>
       <c r="AI18" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AJ18" t="n">
-        <v>4.3</v>
+        <v>0.2</v>
       </c>
       <c r="AK18" t="inlineStr"/>
       <c r="AL18" t="inlineStr"/>
@@ -3176,18 +3158,22 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>PHI</t>
+          <t>CLE</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Tobias Harris</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr"/>
+          <t>Donovan Mitchell</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Out</t>
+        </is>
+      </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>G</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -3196,83 +3182,83 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>28.8</v>
+        <v>38.4</v>
       </c>
       <c r="G19" t="n">
-        <v>27.7</v>
+        <v>41.1</v>
       </c>
       <c r="H19" t="n">
-        <v>28.7</v>
+        <v>39.9</v>
       </c>
       <c r="I19" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J19" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K19" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L19" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M19" t="n">
-        <v>1</v>
-      </c>
-      <c r="N19" t="n">
-        <v>39</v>
-      </c>
-      <c r="O19" t="n">
-        <v>59</v>
-      </c>
-      <c r="P19" t="n">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="Q19" t="n">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="R19" t="n">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="S19" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="T19" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="U19" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="V19" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="V19" t="n">
+        <v>27</v>
       </c>
       <c r="W19" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="X19" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="X19" t="n">
+        <v>37</v>
       </c>
       <c r="Y19" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="Z19" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="Z19" t="n">
+        <v>61</v>
       </c>
       <c r="AA19" t="inlineStr">
         <is>
@@ -3281,101 +3267,113 @@
       </c>
       <c r="AB19" t="inlineStr">
         <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="AC19" t="inlineStr">
+        <is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="AD19" t="inlineStr">
+        <is>
+          <t>BKN</t>
+        </is>
+      </c>
+      <c r="AE19" t="inlineStr">
+        <is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="AF19" t="inlineStr">
+        <is>
+          <t>PHX</t>
+        </is>
+      </c>
+      <c r="AG19" t="inlineStr">
+        <is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="AH19" t="inlineStr">
+        <is>
           <t>NOP</t>
         </is>
       </c>
-      <c r="AC19" t="inlineStr">
-        <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="AD19" t="inlineStr">
-        <is>
-          <t>NYK</t>
-        </is>
-      </c>
-      <c r="AE19" t="inlineStr">
-        <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="AF19" t="inlineStr">
-        <is>
-          <t>NYK</t>
-        </is>
-      </c>
-      <c r="AG19" t="inlineStr">
-        <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="AH19" t="inlineStr">
-        <is>
-          <t>MIL</t>
-        </is>
-      </c>
       <c r="AI19" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AJ19" t="n">
-        <v>0.4</v>
+        <v>-3.8</v>
       </c>
       <c r="AK19" t="n">
-        <v>2.8</v>
+        <v>-13.3</v>
       </c>
       <c r="AL19" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>LAC</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Paul George</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr"/>
+          <t>Trae Young</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Out</t>
+        </is>
+      </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>F</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr"/>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
       <c r="F20" t="n">
-        <v>22.8</v>
+        <v>25.4</v>
       </c>
       <c r="G20" t="n">
-        <v>23.5</v>
+        <v>35</v>
       </c>
       <c r="H20" t="n">
-        <v>30.4</v>
+        <v>37.6</v>
       </c>
       <c r="I20" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="J20" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K20" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L20" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M20" t="n">
         <v>1</v>
       </c>
-      <c r="N20" t="n">
-        <v>9</v>
-      </c>
-      <c r="O20" t="n">
-        <v>33</v>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="P20" t="inlineStr">
         <is>
@@ -3387,17 +3385,19 @@
           <t>-</t>
         </is>
       </c>
-      <c r="R20" t="n">
-        <v>15</v>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="S20" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="T20" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>CLE</t>
         </is>
       </c>
       <c r="U20" t="inlineStr">
@@ -3406,36 +3406,32 @@
         </is>
       </c>
       <c r="V20" t="n">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="W20" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="X20" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="X20" t="n">
+        <v>54</v>
       </c>
       <c r="Y20" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="Z20" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="Z20" t="n">
+        <v>14</v>
       </c>
       <c r="AA20" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AB20" t="inlineStr">
         <is>
-          <t>CHI</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="AC20" t="inlineStr">
@@ -3445,17 +3441,17 @@
       </c>
       <c r="AD20" t="inlineStr">
         <is>
-          <t>MIL</t>
+          <t>NOP</t>
         </is>
       </c>
       <c r="AE20" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AF20" t="inlineStr">
         <is>
-          <t>MIN</t>
+          <t>POR</t>
         </is>
       </c>
       <c r="AG20" t="inlineStr">
@@ -3465,32 +3461,40 @@
       </c>
       <c r="AH20" t="inlineStr">
         <is>
-          <t>CHI</t>
+          <t>UTA</t>
         </is>
       </c>
       <c r="AI20" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AJ20" t="n">
-        <v>-0.6</v>
-      </c>
-      <c r="AK20" t="inlineStr"/>
-      <c r="AL20" t="inlineStr"/>
+        <v>-0.8</v>
+      </c>
+      <c r="AK20" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="AL20" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>PHI</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Fred VanVleet</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr"/>
+          <t>Tyrese Maxey</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Out</t>
+        </is>
+      </c>
       <c r="D21" t="inlineStr">
         <is>
           <t>G</t>
@@ -3502,43 +3506,45 @@
         </is>
       </c>
       <c r="F21" t="n">
-        <v>24.6</v>
+        <v>37.8</v>
       </c>
       <c r="G21" t="n">
-        <v>22.5</v>
+        <v>34.7</v>
       </c>
       <c r="H21" t="n">
-        <v>26.2</v>
+        <v>35.9</v>
       </c>
       <c r="I21" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="J21" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K21" t="n">
         <v>1</v>
       </c>
       <c r="L21" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M21" t="n">
-        <v>1</v>
-      </c>
-      <c r="N21" t="n">
+        <v>5</v>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O21" t="n">
+        <v>32</v>
+      </c>
+      <c r="P21" t="n">
+        <v>44</v>
+      </c>
+      <c r="Q21" t="n">
         <v>42</v>
       </c>
-      <c r="O21" t="n">
-        <v>30</v>
-      </c>
-      <c r="P21" t="n">
-        <v>-2</v>
-      </c>
-      <c r="Q21" t="n">
-        <v>21</v>
-      </c>
       <c r="R21" t="n">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="S21" t="inlineStr">
         <is>
@@ -3547,16 +3553,18 @@
       </c>
       <c r="T21" t="inlineStr">
         <is>
-          <t>LAC</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="U21" t="inlineStr">
         <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="V21" t="n">
-        <v>38</v>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="V21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="W21" t="inlineStr">
         <is>
@@ -3580,12 +3588,12 @@
       </c>
       <c r="AA21" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AB21" t="inlineStr">
         <is>
-          <t>POR</t>
+          <t>NOP</t>
         </is>
       </c>
       <c r="AC21" t="inlineStr">
@@ -3595,7 +3603,7 @@
       </c>
       <c r="AD21" t="inlineStr">
         <is>
-          <t>SAC</t>
+          <t>NYK</t>
         </is>
       </c>
       <c r="AE21" t="inlineStr">
@@ -3605,17 +3613,17 @@
       </c>
       <c r="AF21" t="inlineStr">
         <is>
-          <t>SAS</t>
+          <t>NYK</t>
         </is>
       </c>
       <c r="AG21" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AH21" t="inlineStr">
         <is>
-          <t>WAS</t>
+          <t>MIL</t>
         </is>
       </c>
       <c r="AI21" t="inlineStr">
@@ -3624,71 +3632,79 @@
         </is>
       </c>
       <c r="AJ21" t="n">
-        <v>-0.7</v>
+        <v>-0.2</v>
       </c>
       <c r="AK21" t="n">
-        <v>-5.9</v>
+        <v>-8.800000000000001</v>
       </c>
       <c r="AL21" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>OKC</t>
+          <t>CLE</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Gordon Hayward</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr"/>
+          <t>Evan Mobley</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Out</t>
+        </is>
+      </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>F</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr"/>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
       <c r="F22" t="n">
-        <v>6.2</v>
+        <v>32.4</v>
       </c>
       <c r="G22" t="n">
-        <v>17.7</v>
+        <v>33.3</v>
       </c>
       <c r="H22" t="n">
-        <v>20.1</v>
+        <v>32.2</v>
       </c>
       <c r="I22" t="n">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="J22" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="K22" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L22" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M22" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N22" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="O22" t="n">
-        <v>-1</v>
+        <v>30</v>
       </c>
       <c r="P22" t="n">
-        <v>9</v>
+        <v>54</v>
       </c>
       <c r="Q22" t="n">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="R22" t="n">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="S22" t="inlineStr">
         <is>
@@ -3697,18 +3713,16 @@
       </c>
       <c r="T22" t="inlineStr">
         <is>
-          <t>POR</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="U22" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="V22" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="V22" t="n">
+        <v>49</v>
       </c>
       <c r="W22" t="inlineStr">
         <is>
@@ -3737,7 +3751,7 @@
       </c>
       <c r="AB22" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>MIN</t>
         </is>
       </c>
       <c r="AC22" t="inlineStr">
@@ -3747,7 +3761,7 @@
       </c>
       <c r="AD22" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>BKN</t>
         </is>
       </c>
       <c r="AE22" t="inlineStr">
@@ -3757,17 +3771,17 @@
       </c>
       <c r="AF22" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>PHX</t>
         </is>
       </c>
       <c r="AG22" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AH22" t="inlineStr">
         <is>
-          <t>DAL</t>
+          <t>NOP</t>
         </is>
       </c>
       <c r="AI22" t="inlineStr">
@@ -3776,20 +3790,24 @@
         </is>
       </c>
       <c r="AJ22" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="AK22" t="inlineStr"/>
-      <c r="AL22" t="inlineStr"/>
+        <v>2.2</v>
+      </c>
+      <c r="AK22" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="AL22" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>POR</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Trae Young</t>
+          <t>Deandre Ayton</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -3799,28 +3817,24 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>G</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>O</t>
-        </is>
-      </c>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr"/>
       <c r="F23" t="n">
-        <v>25.4</v>
+        <v>36.4</v>
       </c>
       <c r="G23" t="n">
-        <v>35</v>
+        <v>33.2</v>
       </c>
       <c r="H23" t="n">
-        <v>37.6</v>
+        <v>29.2</v>
       </c>
       <c r="I23" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J23" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K23" t="n">
         <v>1</v>
@@ -3829,7 +3843,7 @@
         <v>1</v>
       </c>
       <c r="M23" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N23" t="inlineStr">
         <is>
@@ -3846,13 +3860,11 @@
           <t>-</t>
         </is>
       </c>
-      <c r="Q23" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="Q23" t="n">
+        <v>28</v>
       </c>
       <c r="R23" t="n">
-        <v>10</v>
+        <v>57</v>
       </c>
       <c r="S23" t="inlineStr">
         <is>
@@ -3861,41 +3873,43 @@
       </c>
       <c r="T23" t="inlineStr">
         <is>
-          <t>CLE</t>
+          <t>OKC</t>
         </is>
       </c>
       <c r="U23" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="V23" t="n">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="W23" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="X23" t="n">
-        <v>54</v>
+        <v>21</v>
       </c>
       <c r="Y23" t="inlineStr">
         <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="Z23" t="n">
-        <v>14</v>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Z23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="AA23" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AB23" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="AC23" t="inlineStr">
@@ -3905,27 +3919,27 @@
       </c>
       <c r="AD23" t="inlineStr">
         <is>
-          <t>NOP</t>
+          <t>TOR</t>
         </is>
       </c>
       <c r="AE23" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AF23" t="inlineStr">
         <is>
-          <t>POR</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="AG23" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AH23" t="inlineStr">
         <is>
-          <t>UTA</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="AI23" t="inlineStr">
@@ -3934,14 +3948,10 @@
         </is>
       </c>
       <c r="AJ23" t="n">
-        <v>-0.8</v>
-      </c>
-      <c r="AK23" t="n">
-        <v>1.8</v>
-      </c>
-      <c r="AL23" t="n">
-        <v>8</v>
-      </c>
+        <v>0.5</v>
+      </c>
+      <c r="AK23" t="inlineStr"/>
+      <c r="AL23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -3975,13 +3985,13 @@
         <v>35</v>
       </c>
       <c r="I24" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J24" t="n">
         <v>1</v>
       </c>
       <c r="K24" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L24" t="n">
         <v>1</v>
@@ -3989,20 +3999,22 @@
       <c r="M24" t="n">
         <v>3</v>
       </c>
-      <c r="N24" t="n">
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O24" t="n">
         <v>41</v>
       </c>
-      <c r="O24" t="n">
+      <c r="P24" t="n">
         <v>21</v>
       </c>
-      <c r="P24" t="n">
+      <c r="Q24" t="n">
         <v>4</v>
       </c>
-      <c r="Q24" t="n">
+      <c r="R24" t="n">
         <v>44</v>
-      </c>
-      <c r="R24" t="n">
-        <v>33</v>
       </c>
       <c r="S24" t="inlineStr">
         <is>
@@ -4096,12 +4108,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>GSW</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Andrew Wiggins</t>
+          <t>Jaren Jackson Jr.</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -4111,33 +4123,33 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>C</t>
         </is>
       </c>
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="n">
-        <v>25.4</v>
+        <v>30.4</v>
       </c>
       <c r="G25" t="n">
-        <v>25.1</v>
+        <v>30.5</v>
       </c>
       <c r="H25" t="n">
-        <v>17.8</v>
+        <v>30.5</v>
       </c>
       <c r="I25" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="J25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K25" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L25" t="n">
         <v>2</v>
       </c>
       <c r="M25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N25" t="inlineStr">
         <is>
@@ -4154,31 +4166,31 @@
           <t>-</t>
         </is>
       </c>
-      <c r="Q25" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="Q25" t="n">
+        <v>50</v>
       </c>
       <c r="R25" t="n">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="S25" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="T25" t="inlineStr">
         <is>
-          <t>MIL</t>
+          <t>PHI</t>
         </is>
       </c>
       <c r="U25" t="inlineStr">
         <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="V25" t="n">
-        <v>4</v>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="V25" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="W25" t="inlineStr">
         <is>
@@ -4207,46 +4219,46 @@
       </c>
       <c r="AB25" t="inlineStr">
         <is>
-          <t>CHI</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="AC25" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AD25" t="inlineStr">
         <is>
-          <t>SAS</t>
+          <t>OKC</t>
         </is>
       </c>
       <c r="AE25" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AF25" t="inlineStr">
         <is>
-          <t>SAS</t>
+          <t>WAS</t>
         </is>
       </c>
       <c r="AG25" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AH25" t="inlineStr">
         <is>
-          <t>DAL</t>
+          <t>CHA</t>
         </is>
       </c>
       <c r="AI25" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AJ25" t="n">
-        <v>-0.5</v>
+        <v>2.4</v>
       </c>
       <c r="AK25" t="inlineStr"/>
       <c r="AL25" t="inlineStr"/>
@@ -4443,13 +4455,13 @@
         <v>18.7</v>
       </c>
       <c r="I27" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="J27" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L27" t="n">
         <v>0</v>
@@ -4462,17 +4474,19 @@
           <t>-</t>
         </is>
       </c>
-      <c r="O27" t="n">
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P27" t="n">
         <v>10</v>
       </c>
-      <c r="P27" t="n">
+      <c r="Q27" t="n">
         <v>12</v>
       </c>
-      <c r="Q27" t="n">
+      <c r="R27" t="n">
         <v>10</v>
-      </c>
-      <c r="R27" t="n">
-        <v>8</v>
       </c>
       <c r="S27" t="inlineStr">
         <is>

</xml_diff>